<commit_message>
edições para trabalhar no caos
</commit_message>
<xml_diff>
--- a/97_enquete/1.xlsx
+++ b/97_enquete/1.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomaz\OneDrive\Documentos\Tomaz\UFRJ\Mestrado\Introducao ao R\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31140" windowHeight="14800"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -71,16 +69,16 @@
     <t>Ouvindo/Depto Ecologia/Labvert</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>No laboratório através da profa Camila</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -224,7 +222,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -418,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -429,12 +427,23 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -486,7 +495,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -495,10 +504,15 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>